<commit_message>
updated entry with closet and window
</commit_message>
<xml_diff>
--- a/itemized/1424_trygg_ely_itemized_windows_2024-01-16.xlsx
+++ b/itemized/1424_trygg_ely_itemized_windows_2024-01-16.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deniselive\Documents\johnson-family-cabin\itemized\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2927ACC2-1BF6-4717-9F39-D39AE1F8184C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="495" windowWidth="24105" windowHeight="15705" tabRatio="500"/>
+    <workbookView xWindow="1560" yWindow="15" windowWidth="24105" windowHeight="15705" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MARVIN WINDOWS" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'MARVIN WINDOWS'!$A$1:$I$16</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -137,6 +143,9 @@
     <t>BHJ Reference</t>
   </si>
   <si>
+    <t>Cabin items Marvin 3.xlsx</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -145,7 +154,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>4' 0</t>
+      <t>4' 1</t>
     </r>
     <r>
       <rPr>
@@ -157,14 +166,11 @@
       <t>" W x 5' 11 5/8" H</t>
     </r>
   </si>
-  <si>
-    <t>Cabin items Marvin 3.xlsx</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -314,12 +320,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -332,6 +332,12 @@
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="28">
@@ -698,7 +704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="150" workbookViewId="0"/>
@@ -712,8 +718,8 @@
     <col min="5" max="5" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.875" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -746,10 +752,10 @@
       <c r="G3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="15" t="s">
         <v>27</v>
       </c>
     </row>
@@ -775,10 +781,10 @@
       <c r="G4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="16">
         <v>3115.2</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="16">
         <f>E4*H4</f>
         <v>3115.2</v>
       </c>
@@ -805,10 +811,10 @@
       <c r="G5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="16">
         <v>3115.2</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="16">
         <f t="shared" ref="I5:I11" si="0">E5*H5</f>
         <v>3115.2</v>
       </c>
@@ -833,10 +839,10 @@
         <v>4</v>
       </c>
       <c r="G6" s="8"/>
-      <c r="H6" s="18">
+      <c r="H6" s="16">
         <v>763.2</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="16">
         <f t="shared" si="0"/>
         <v>763.2</v>
       </c>
@@ -861,10 +867,10 @@
         <v>4</v>
       </c>
       <c r="G7" s="8"/>
-      <c r="H7" s="18">
+      <c r="H7" s="16">
         <v>1108.8</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="16">
         <f t="shared" si="0"/>
         <v>1108.8</v>
       </c>
@@ -889,10 +895,10 @@
         <v>4</v>
       </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="18">
+      <c r="H8" s="16">
         <v>1108.8</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="16">
         <f t="shared" ref="I8" si="1">E8*H8</f>
         <v>1108.8</v>
       </c>
@@ -901,8 +907,8 @@
       <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>34</v>
+      <c r="B9" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>18</v>
@@ -917,10 +923,10 @@
         <v>4</v>
       </c>
       <c r="G9" s="8"/>
-      <c r="H9" s="18">
+      <c r="H9" s="16">
         <v>1108.8</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="16">
         <f t="shared" si="0"/>
         <v>1108.8</v>
       </c>
@@ -947,10 +953,10 @@
       <c r="G10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="16">
         <v>1158.4000000000001</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="16">
         <f t="shared" si="0"/>
         <v>1158.4000000000001</v>
       </c>
@@ -967,11 +973,11 @@
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="18">
+      <c r="H11" s="16">
         <f>0.07375*I10</f>
         <v>85.432000000000002</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="16">
         <f t="shared" si="0"/>
         <v>85.432000000000002</v>
       </c>
@@ -986,23 +992,23 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19">
+      <c r="H12" s="17"/>
+      <c r="I12" s="17">
         <f>SUM(I4:I11)</f>
         <v>11563.831999999999</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="14"/>
+      <c r="A16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>